<commit_message>
my diary and Server class diagram
</commit_message>
<xml_diff>
--- a/Journaux_de_travail/Daniel.xlsx
+++ b/Journaux_de_travail/Daniel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -45,10 +45,22 @@
      - etc</t>
   </si>
   <si>
-    <t>- Test de l'application et de ses fonctionnalités</t>
-  </si>
-  <si>
-    <t>- Modification des règles du jeu sur le repo distant</t>
+    <t>Modification des règles du jeu sur le repo distant</t>
+  </si>
+  <si>
+    <t>Test simple de l'application et de ses fonctionnalités</t>
+  </si>
+  <si>
+    <t>Analyse de l'application : partie simple</t>
+  </si>
+  <si>
+    <t>Analyse de l'application : partie tournoi</t>
+  </si>
+  <si>
+    <t>Diagramme de classe côté serveur</t>
+  </si>
+  <si>
+    <t>Début diagramme de classe (serveur, client et common)</t>
   </si>
 </sst>
 </file>
@@ -478,7 +490,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +539,7 @@
         <v>42999</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="6">
         <v>0.5</v>
@@ -538,31 +550,55 @@
         <v>42999</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>43004</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>43008</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="6"/>
-    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="6"/>
+      <c r="A10" s="3">
+        <v>43011</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="3">
+        <v>43016</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -670,7 +706,7 @@
       </c>
       <c r="C32" s="7">
         <f>SUM(C5:C31)</f>
-        <v>4.5</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update my work diary
</commit_message>
<xml_diff>
--- a/Journaux_de_travail/Daniel.xlsx
+++ b/Journaux_de_travail/Daniel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEIG-A3S1\PDG\HEIG-2017-PDG-WORDOFF\Journaux_de_travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -96,21 +96,12 @@
 </t>
   </si>
   <si>
-    <t>Ajout de getter et setter intelligent dans la classe Side</t>
-  </si>
-  <si>
     <t>Refactoring des modèles existants dans les modules Common et Server</t>
   </si>
   <si>
     <t>Discussion avec les membres du groupe sur le refactoring a effectué et des adaptations a effectué du côté client</t>
   </si>
   <si>
-    <t>Création d'un service pour le Game</t>
-  </si>
-  <si>
-    <t>Suppression de classe devenue inutile ou redondante</t>
-  </si>
-  <si>
     <t>Refactoring dû aux changements effectués par Antoine, correction de code dû aux erreurs renvoyées et modification des tests du côté serveur (le client sera corrigé demain)</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>Réparation du client afin que le groupe s'occupant de l'interface puisse travailler</t>
   </si>
   <si>
-    <t>Suppression de code redondant ou inutile, modification de constructeur et suppression de la classe PlayerSummaryDto qui sera remplacée une classe liée à l'utilisateur (1 classe pour les stats de l'utilisateur)</t>
-  </si>
-  <si>
     <t>Modification des diagrammes de classes</t>
   </si>
   <si>
@@ -135,13 +123,28 @@
     <t>Ajout de méthodes et d’annotations (spring) pour pouvoir jouer une partie et création des méthodes dans le GameController</t>
   </si>
   <si>
-    <t>Lecture et apprentissage du l’utilisation de spring, de la création de requête HTTP en java et de l'utilisation de hibernate</t>
-  </si>
-  <si>
     <t>Discussion avec les membre du groupe sur l'avancement globale du projet et l'utilisation de spring</t>
   </si>
   <si>
     <t>Rajout d'Exception pour la classe GameService qui sont renvoyé au GameController (le système d'envoi de l'erreur au client sera discuté dans les prochain jours avec Christopher)</t>
+  </si>
+  <si>
+    <t>Lecture et apprentissage du l’utilisation de spring</t>
+  </si>
+  <si>
+    <t>Lecture et apprentissage pour la création de requête HTTP en java et de l'utilisation de hibernate</t>
+  </si>
+  <si>
+    <t>Ajout de getter et setter intelligent dans les modèles</t>
+  </si>
+  <si>
+    <t>Création d'un service qui contiendra la logique du Game</t>
+  </si>
+  <si>
+    <t>Suppression de classes devenues inutiles ou redondantes</t>
+  </si>
+  <si>
+    <t>Suppression de code redondant ou inutile, modification de constructeur et suppression de la classe PlayerSummaryDto qui sera remplacée par une classe liée à l'utilisateur (1 classe pour les stats de l'utilisateur)</t>
   </si>
 </sst>
 </file>
@@ -652,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +784,7 @@
         <v>43018</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="11">
         <v>1</v>
@@ -798,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>43018</v>
       </c>
@@ -858,18 +861,18 @@
         <v>43029</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>43030</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="11">
         <v>5</v>
@@ -880,7 +883,7 @@
         <v>43031</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="14">
         <v>3</v>
@@ -888,54 +891,54 @@
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <v>43032</v>
+        <v>43031</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="11">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>43032</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>43032</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>43033</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>43033</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C26" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>43033</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27" s="11">
         <v>2</v>
@@ -943,60 +946,60 @@
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
+        <v>43033</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
         <v>43039</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="11">
+      <c r="B29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="11">
         <v>3.5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>43044</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>43044</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C30" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>43044</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C31" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>43044</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>43044</v>
       </c>
@@ -1007,31 +1010,38 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
-        <v>43045</v>
+        <v>43044</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C34" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>43045</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C35" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="C36" s="11"/>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>43045</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
@@ -1063,8 +1073,8 @@
         <v>19</v>
       </c>
       <c r="C42" s="13">
-        <f>SUM(C5:C35)</f>
-        <v>58</v>
+        <f>SUM(C5:C36)</f>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>